<commit_message>
update: docs and pcb
</commit_message>
<xml_diff>
--- a/pcb/node/BOM_pa.xlsx
+++ b/pcb/node/BOM_pa.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Luis\gitprojects\precision-agriculture\pcb\node\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C37479E1-AC86-4C51-AD9C-36B8693AE22B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDA55AE0-E6BE-4450-AAFE-1864D21A40FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="90">
   <si>
     <t>xxxx xxxx xxxxx xxPCS BOM  (Sample Bill of Materials)</t>
   </si>
@@ -361,7 +361,22 @@
     <t>https://datasheet.lcsc.com/lcsc/1912111437_SHOU-HAN-TF-PUSH_C393941.pdf</t>
   </si>
   <si>
-    <t>USB C</t>
+    <t>DEALON</t>
+  </si>
+  <si>
+    <t>USB-TYPE-C-019</t>
+  </si>
+  <si>
+    <t>3A 1 Surface Mount 16P Female -25℃~+85℃ Type-C SMD USB Connectors</t>
+  </si>
+  <si>
+    <t>SMD 16P female</t>
+  </si>
+  <si>
+    <t>https://datasheet.lcsc.com/lcsc/2201121330_DEALON-USB-TYPE-C-019_C2927039.pdf</t>
+  </si>
+  <si>
+    <t>https://www.lcsc.com/product-detail/span-style-background-color-ff0-USB-span-Connectors_DEALON-USB-TYPE-C-019_C2927039.html</t>
   </si>
 </sst>
 </file>
@@ -608,7 +623,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -622,9 +637,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
@@ -672,12 +684,8 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -717,18 +725,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
@@ -736,6 +732,24 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1566,7 +1580,7 @@
   <dimension ref="A2:M25"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.25"/>
@@ -1587,306 +1601,318 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:13" ht="19.5" customHeight="1">
-      <c r="A2" s="49"/>
-      <c r="B2" s="49"/>
-      <c r="D2" s="48" t="s">
+      <c r="A2" s="50"/>
+      <c r="B2" s="50"/>
+      <c r="D2" s="49" t="s">
         <v>0</v>
       </c>
-      <c r="E2" s="48"/>
-      <c r="F2" s="48"/>
+      <c r="E2" s="49"/>
+      <c r="F2" s="49"/>
     </row>
     <row r="3" spans="1:13">
-      <c r="A3" s="49"/>
-      <c r="B3" s="49"/>
-      <c r="D3" s="48"/>
-      <c r="E3" s="48"/>
-      <c r="F3" s="48"/>
+      <c r="A3" s="50"/>
+      <c r="B3" s="50"/>
+      <c r="D3" s="49"/>
+      <c r="E3" s="49"/>
+      <c r="F3" s="49"/>
     </row>
     <row r="4" spans="1:13">
-      <c r="D4" s="48"/>
-      <c r="E4" s="48"/>
-      <c r="F4" s="48"/>
+      <c r="D4" s="49"/>
+      <c r="E4" s="49"/>
+      <c r="F4" s="49"/>
     </row>
     <row r="6" spans="1:13" ht="28.5" customHeight="1">
-      <c r="A6" s="13" t="s">
+      <c r="A6" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="14" t="s">
+      <c r="B6" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="15" t="s">
+      <c r="C6" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="D6" s="16" t="s">
+      <c r="D6" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="E6" s="15" t="s">
+      <c r="E6" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="F6" s="16" t="s">
+      <c r="F6" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="G6" s="14" t="s">
+      <c r="G6" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="H6" s="16" t="s">
+      <c r="H6" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="I6" s="17" t="s">
+      <c r="I6" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="J6" s="16" t="s">
+      <c r="J6" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="K6" s="16" t="s">
+      <c r="K6" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="L6" s="16" t="s">
+      <c r="L6" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="M6" s="16" t="s">
+      <c r="M6" s="15" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:13" s="35" customFormat="1">
-      <c r="A7" s="28">
+    <row r="7" spans="1:13" s="32" customFormat="1">
+      <c r="A7" s="25">
         <v>1</v>
       </c>
-      <c r="B7" s="29"/>
-      <c r="C7" s="30">
+      <c r="B7" s="26"/>
+      <c r="C7" s="27">
         <v>1</v>
       </c>
-      <c r="D7" s="29" t="s">
+      <c r="D7" s="26" t="s">
         <v>60</v>
       </c>
-      <c r="E7" s="29" t="s">
+      <c r="E7" s="26" t="s">
         <v>61</v>
       </c>
-      <c r="F7" s="31" t="s">
+      <c r="F7" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="G7" s="31" t="s">
+      <c r="G7" s="28" t="s">
         <v>18</v>
       </c>
-      <c r="H7" s="32" t="s">
+      <c r="H7" s="29" t="s">
         <v>10</v>
       </c>
-      <c r="I7" s="33"/>
-      <c r="J7" s="34" t="s">
+      <c r="I7" s="30"/>
+      <c r="J7" s="31" t="s">
         <v>62</v>
       </c>
-      <c r="K7" s="34" t="s">
+      <c r="K7" s="31" t="s">
         <v>63</v>
       </c>
-      <c r="L7" s="44">
+      <c r="L7" s="41">
         <v>1.4732000000000001</v>
       </c>
     </row>
-    <row r="8" spans="1:13" s="35" customFormat="1">
-      <c r="A8" s="28">
+    <row r="8" spans="1:13" s="32" customFormat="1">
+      <c r="A8" s="25">
         <v>2</v>
       </c>
-      <c r="B8" s="29"/>
-      <c r="C8" s="30">
+      <c r="B8" s="26"/>
+      <c r="C8" s="27">
         <v>1</v>
       </c>
-      <c r="D8" s="29" t="s">
+      <c r="D8" s="26" t="s">
         <v>78</v>
       </c>
-      <c r="E8" s="29" t="s">
+      <c r="E8" s="26" t="s">
         <v>79</v>
       </c>
-      <c r="F8" s="31" t="s">
+      <c r="F8" s="28" t="s">
         <v>80</v>
       </c>
-      <c r="G8" s="31" t="s">
+      <c r="G8" s="28" t="s">
         <v>81</v>
       </c>
-      <c r="H8" s="51" t="s">
+      <c r="H8" s="44" t="s">
         <v>10</v>
       </c>
-      <c r="I8" s="52"/>
-      <c r="J8" s="34" t="s">
+      <c r="I8" s="45"/>
+      <c r="J8" s="31" t="s">
         <v>83</v>
       </c>
-      <c r="K8" s="34" t="s">
+      <c r="K8" s="31" t="s">
         <v>82</v>
       </c>
-      <c r="L8" s="44">
+      <c r="L8" s="41">
         <v>4.5499999999999999E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:13">
-      <c r="A9" s="10"/>
-      <c r="B9" s="4"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="27" t="s">
+    <row r="9" spans="1:13" s="32" customFormat="1">
+      <c r="A9" s="25"/>
+      <c r="B9" s="26"/>
+      <c r="C9" s="27"/>
+      <c r="D9" s="51" t="s">
         <v>84</v>
       </c>
-      <c r="E9" s="4"/>
-      <c r="F9" s="5"/>
-      <c r="G9" s="5"/>
-      <c r="H9" s="25" t="s">
+      <c r="E9" s="26" t="s">
+        <v>85</v>
+      </c>
+      <c r="F9" s="28" t="s">
+        <v>86</v>
+      </c>
+      <c r="G9" s="52" t="s">
+        <v>87</v>
+      </c>
+      <c r="H9" s="29" t="s">
         <v>10</v>
       </c>
-      <c r="I9" s="11"/>
-      <c r="J9" s="26"/>
-      <c r="K9" s="26"/>
-      <c r="L9" s="43"/>
+      <c r="I9" s="30"/>
+      <c r="J9" s="31" t="s">
+        <v>88</v>
+      </c>
+      <c r="K9" s="31" t="s">
+        <v>89</v>
+      </c>
+      <c r="L9" s="41">
+        <v>0.45</v>
+      </c>
     </row>
-    <row r="10" spans="1:13" s="35" customFormat="1">
-      <c r="A10" s="28"/>
-      <c r="B10" s="29"/>
-      <c r="C10" s="30"/>
-      <c r="D10" s="29" t="s">
+    <row r="10" spans="1:13" s="32" customFormat="1">
+      <c r="A10" s="25"/>
+      <c r="B10" s="26"/>
+      <c r="C10" s="27"/>
+      <c r="D10" s="26" t="s">
         <v>19</v>
       </c>
-      <c r="E10" s="29" t="s">
+      <c r="E10" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="F10" s="31" t="s">
+      <c r="F10" s="28" t="s">
         <v>21</v>
       </c>
-      <c r="G10" s="31" t="s">
+      <c r="G10" s="28" t="s">
         <v>22</v>
       </c>
-      <c r="H10" s="32" t="s">
+      <c r="H10" s="29" t="s">
         <v>10</v>
       </c>
-      <c r="I10" s="33"/>
-      <c r="J10" s="34" t="s">
+      <c r="I10" s="30"/>
+      <c r="J10" s="31" t="s">
         <v>24</v>
       </c>
-      <c r="K10" s="34" t="s">
+      <c r="K10" s="31" t="s">
         <v>23</v>
       </c>
-      <c r="L10" s="44">
+      <c r="L10" s="41">
         <v>1.95</v>
       </c>
     </row>
-    <row r="11" spans="1:13" s="35" customFormat="1">
-      <c r="A11" s="28"/>
-      <c r="B11" s="29"/>
-      <c r="C11" s="30"/>
-      <c r="D11" s="29" t="s">
+    <row r="11" spans="1:13" s="32" customFormat="1">
+      <c r="A11" s="25"/>
+      <c r="B11" s="26"/>
+      <c r="C11" s="27"/>
+      <c r="D11" s="26" t="s">
         <v>25</v>
       </c>
-      <c r="E11" s="29" t="s">
+      <c r="E11" s="26" t="s">
         <v>70</v>
       </c>
-      <c r="F11" s="31" t="s">
+      <c r="F11" s="28" t="s">
         <v>26</v>
       </c>
-      <c r="G11" s="31" t="s">
+      <c r="G11" s="28" t="s">
         <v>27</v>
       </c>
-      <c r="H11" s="32" t="s">
+      <c r="H11" s="29" t="s">
         <v>10</v>
       </c>
-      <c r="I11" s="33"/>
-      <c r="J11" s="34" t="s">
+      <c r="I11" s="30"/>
+      <c r="J11" s="31" t="s">
         <v>72</v>
       </c>
-      <c r="K11" s="34" t="s">
+      <c r="K11" s="31" t="s">
         <v>71</v>
       </c>
-      <c r="L11" s="44">
+      <c r="L11" s="41">
         <v>4.8856999999999999</v>
       </c>
     </row>
-    <row r="12" spans="1:13" s="35" customFormat="1">
-      <c r="A12" s="28"/>
-      <c r="B12" s="29"/>
-      <c r="C12" s="30"/>
-      <c r="D12" s="29" t="s">
+    <row r="12" spans="1:13" s="32" customFormat="1">
+      <c r="A12" s="25"/>
+      <c r="B12" s="26"/>
+      <c r="C12" s="27"/>
+      <c r="D12" s="26" t="s">
         <v>28</v>
       </c>
-      <c r="E12" s="29" t="s">
+      <c r="E12" s="26" t="s">
         <v>29</v>
       </c>
-      <c r="F12" s="31" t="s">
+      <c r="F12" s="28" t="s">
         <v>30</v>
       </c>
-      <c r="G12" s="36" t="s">
+      <c r="G12" s="33" t="s">
         <v>31</v>
       </c>
-      <c r="H12" s="32" t="s">
+      <c r="H12" s="29" t="s">
         <v>10</v>
       </c>
-      <c r="I12" s="33"/>
-      <c r="J12" s="34" t="s">
+      <c r="I12" s="30"/>
+      <c r="J12" s="31" t="s">
         <v>32</v>
       </c>
-      <c r="K12" s="34" t="s">
+      <c r="K12" s="31" t="s">
         <v>33</v>
       </c>
-      <c r="L12" s="44">
+      <c r="L12" s="41">
         <v>9.6</v>
       </c>
     </row>
-    <row r="13" spans="1:13" s="35" customFormat="1">
-      <c r="A13" s="28"/>
-      <c r="B13" s="29"/>
-      <c r="C13" s="30"/>
-      <c r="D13" s="29" t="s">
+    <row r="13" spans="1:13" s="32" customFormat="1">
+      <c r="A13" s="25"/>
+      <c r="B13" s="26"/>
+      <c r="C13" s="27"/>
+      <c r="D13" s="26" t="s">
         <v>34</v>
       </c>
-      <c r="E13" s="29" t="s">
+      <c r="E13" s="26" t="s">
         <v>35</v>
       </c>
-      <c r="F13" s="31" t="s">
+      <c r="F13" s="28" t="s">
         <v>36</v>
       </c>
-      <c r="G13" s="36" t="s">
+      <c r="G13" s="33" t="s">
         <v>37</v>
       </c>
-      <c r="H13" s="32" t="s">
+      <c r="H13" s="29" t="s">
         <v>10</v>
       </c>
-      <c r="I13" s="33"/>
-      <c r="J13" s="34" t="s">
+      <c r="I13" s="30"/>
+      <c r="J13" s="31" t="s">
         <v>38</v>
       </c>
-      <c r="K13" s="34" t="s">
+      <c r="K13" s="31" t="s">
         <v>39</v>
       </c>
-      <c r="L13" s="44">
+      <c r="L13" s="41">
         <v>4.9400000000000004</v>
       </c>
     </row>
-    <row r="14" spans="1:13" s="35" customFormat="1" ht="15">
-      <c r="A14" s="28"/>
-      <c r="B14" s="29"/>
-      <c r="C14" s="30"/>
-      <c r="D14" s="37" t="s">
+    <row r="14" spans="1:13" s="32" customFormat="1" ht="15">
+      <c r="A14" s="25"/>
+      <c r="B14" s="26"/>
+      <c r="C14" s="27"/>
+      <c r="D14" s="34" t="s">
         <v>40</v>
       </c>
-      <c r="E14" s="37" t="s">
+      <c r="E14" s="34" t="s">
         <v>41</v>
       </c>
-      <c r="F14" s="38" t="s">
+      <c r="F14" s="35" t="s">
         <v>42</v>
       </c>
-      <c r="G14" s="38" t="s">
+      <c r="G14" s="35" t="s">
         <v>43</v>
       </c>
-      <c r="H14" s="39" t="s">
+      <c r="H14" s="36" t="s">
         <v>44</v>
       </c>
-      <c r="I14" s="40"/>
-      <c r="J14" s="41" t="s">
+      <c r="I14" s="37"/>
+      <c r="J14" s="38" t="s">
         <v>45</v>
       </c>
-      <c r="K14" s="42" t="s">
+      <c r="K14" s="39" t="s">
         <v>46</v>
       </c>
-      <c r="L14" s="45">
+      <c r="L14" s="42">
         <v>0.27</v>
       </c>
-      <c r="M14" s="50"/>
+      <c r="M14" s="43"/>
     </row>
     <row r="15" spans="1:13">
-      <c r="A15" s="10"/>
+      <c r="A15" s="9"/>
       <c r="B15" s="4"/>
       <c r="C15" s="3"/>
       <c r="D15" s="4" t="s">
@@ -1898,176 +1924,176 @@
       <c r="F15" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="G15" s="8" t="s">
+      <c r="G15" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="H15" s="7" t="s">
+      <c r="H15" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="I15" s="12"/>
-      <c r="J15" s="26" t="s">
+      <c r="I15" s="11"/>
+      <c r="J15" s="24" t="s">
         <v>52</v>
       </c>
-      <c r="K15" s="26" t="s">
+      <c r="K15" s="24" t="s">
         <v>53</v>
       </c>
-      <c r="L15" s="43">
+      <c r="L15" s="40">
         <v>6.9</v>
       </c>
     </row>
-    <row r="16" spans="1:13" s="35" customFormat="1">
-      <c r="A16" s="28"/>
-      <c r="B16" s="29"/>
-      <c r="C16" s="30"/>
-      <c r="D16" s="29" t="s">
+    <row r="16" spans="1:13" s="32" customFormat="1">
+      <c r="A16" s="25"/>
+      <c r="B16" s="26"/>
+      <c r="C16" s="27"/>
+      <c r="D16" s="26" t="s">
         <v>54</v>
       </c>
-      <c r="E16" s="29" t="s">
+      <c r="E16" s="26" t="s">
         <v>55</v>
       </c>
-      <c r="F16" s="29" t="s">
+      <c r="F16" s="26" t="s">
         <v>56</v>
       </c>
-      <c r="G16" s="36" t="s">
+      <c r="G16" s="33" t="s">
         <v>57</v>
       </c>
-      <c r="H16" s="32" t="s">
+      <c r="H16" s="29" t="s">
         <v>10</v>
       </c>
-      <c r="I16" s="33"/>
-      <c r="J16" s="34" t="s">
+      <c r="I16" s="30"/>
+      <c r="J16" s="31" t="s">
         <v>58</v>
       </c>
-      <c r="K16" s="34" t="s">
+      <c r="K16" s="31" t="s">
         <v>59</v>
       </c>
-      <c r="L16" s="44">
+      <c r="L16" s="41">
         <v>2.2700000000000001E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:12" s="35" customFormat="1">
-      <c r="A17" s="28"/>
-      <c r="B17" s="29"/>
-      <c r="C17" s="30"/>
-      <c r="D17" s="29" t="s">
+    <row r="17" spans="1:12" s="32" customFormat="1">
+      <c r="A17" s="25"/>
+      <c r="B17" s="26"/>
+      <c r="C17" s="27"/>
+      <c r="D17" s="26" t="s">
         <v>64</v>
       </c>
-      <c r="E17" s="29" t="s">
+      <c r="E17" s="26" t="s">
         <v>65</v>
       </c>
-      <c r="F17" s="31" t="s">
+      <c r="F17" s="28" t="s">
         <v>67</v>
       </c>
-      <c r="G17" s="36" t="s">
+      <c r="G17" s="33" t="s">
         <v>66</v>
       </c>
-      <c r="H17" s="32" t="s">
+      <c r="H17" s="29" t="s">
         <v>10</v>
       </c>
-      <c r="I17" s="33"/>
-      <c r="J17" s="34" t="s">
+      <c r="I17" s="30"/>
+      <c r="J17" s="31" t="s">
         <v>68</v>
       </c>
-      <c r="K17" s="34" t="s">
+      <c r="K17" s="31" t="s">
         <v>69</v>
       </c>
-      <c r="L17" s="44">
+      <c r="L17" s="41">
         <v>3.9199999999999999E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:12" s="35" customFormat="1">
-      <c r="A18" s="28"/>
-      <c r="B18" s="29"/>
-      <c r="C18" s="30"/>
-      <c r="D18" s="29" t="s">
+    <row r="18" spans="1:12" s="32" customFormat="1">
+      <c r="A18" s="25"/>
+      <c r="B18" s="26"/>
+      <c r="C18" s="27"/>
+      <c r="D18" s="26" t="s">
         <v>28</v>
       </c>
-      <c r="E18" s="29" t="s">
+      <c r="E18" s="26" t="s">
         <v>73</v>
       </c>
-      <c r="F18" s="29" t="s">
+      <c r="F18" s="26" t="s">
         <v>74</v>
       </c>
-      <c r="G18" s="36" t="s">
+      <c r="G18" s="33" t="s">
         <v>75</v>
       </c>
-      <c r="H18" s="32" t="s">
+      <c r="H18" s="29" t="s">
         <v>10</v>
       </c>
-      <c r="I18" s="33"/>
-      <c r="J18" s="34" t="s">
+      <c r="I18" s="30"/>
+      <c r="J18" s="31" t="s">
         <v>76</v>
       </c>
-      <c r="K18" s="34" t="s">
+      <c r="K18" s="31" t="s">
         <v>77</v>
       </c>
-      <c r="L18" s="44">
+      <c r="L18" s="41">
         <v>0.49959999999999999</v>
       </c>
     </row>
     <row r="19" spans="1:12">
-      <c r="A19" s="10"/>
+      <c r="A19" s="9"/>
       <c r="B19" s="4"/>
       <c r="C19" s="3"/>
       <c r="D19" s="4"/>
       <c r="E19" s="4"/>
       <c r="F19" s="4"/>
-      <c r="G19" s="8"/>
-      <c r="H19" s="6"/>
-      <c r="I19" s="11"/>
-      <c r="L19" s="43"/>
+      <c r="G19" s="7"/>
+      <c r="H19" s="5"/>
+      <c r="I19" s="10"/>
+      <c r="L19" s="40"/>
     </row>
     <row r="20" spans="1:12">
-      <c r="A20" s="18"/>
-      <c r="B20" s="19"/>
-      <c r="C20" s="20"/>
-      <c r="D20" s="19"/>
-      <c r="E20" s="19"/>
-      <c r="F20" s="21"/>
-      <c r="G20" s="22"/>
-      <c r="H20" s="23"/>
-      <c r="I20" s="24"/>
-      <c r="L20" s="43"/>
+      <c r="A20" s="17"/>
+      <c r="B20" s="18"/>
+      <c r="C20" s="19"/>
+      <c r="D20" s="18"/>
+      <c r="E20" s="18"/>
+      <c r="F20" s="20"/>
+      <c r="G20" s="21"/>
+      <c r="H20" s="22"/>
+      <c r="I20" s="23"/>
+      <c r="L20" s="40"/>
     </row>
     <row r="21" spans="1:12">
-      <c r="G21" s="53"/>
+      <c r="G21" s="46"/>
     </row>
     <row r="23" spans="1:12">
-      <c r="A23" s="46" t="s">
+      <c r="A23" s="47" t="s">
         <v>11</v>
       </c>
-      <c r="B23" s="46"/>
-      <c r="C23" s="46"/>
-      <c r="D23" s="46"/>
-      <c r="E23" s="46"/>
-      <c r="F23" s="46"/>
-      <c r="G23" s="46"/>
-      <c r="H23" s="46"/>
-      <c r="I23" s="46"/>
+      <c r="B23" s="47"/>
+      <c r="C23" s="47"/>
+      <c r="D23" s="47"/>
+      <c r="E23" s="47"/>
+      <c r="F23" s="47"/>
+      <c r="G23" s="47"/>
+      <c r="H23" s="47"/>
+      <c r="I23" s="47"/>
     </row>
     <row r="24" spans="1:12">
-      <c r="A24" s="9"/>
-      <c r="B24" s="9"/>
-      <c r="C24" s="9"/>
-      <c r="D24" s="9"/>
-      <c r="E24" s="9"/>
-      <c r="F24" s="9"/>
-      <c r="G24" s="9"/>
-      <c r="H24" s="9"/>
-      <c r="I24" s="9"/>
+      <c r="A24" s="8"/>
+      <c r="B24" s="8"/>
+      <c r="C24" s="8"/>
+      <c r="D24" s="8"/>
+      <c r="E24" s="8"/>
+      <c r="F24" s="8"/>
+      <c r="G24" s="8"/>
+      <c r="H24" s="8"/>
+      <c r="I24" s="8"/>
     </row>
     <row r="25" spans="1:12" s="2" customFormat="1" ht="13.5">
-      <c r="A25" s="47" t="s">
+      <c r="A25" s="48" t="s">
         <v>12</v>
       </c>
-      <c r="B25" s="47"/>
-      <c r="C25" s="47"/>
-      <c r="D25" s="47"/>
-      <c r="E25" s="47"/>
-      <c r="F25" s="47"/>
-      <c r="G25" s="47"/>
-      <c r="H25" s="47"/>
-      <c r="I25" s="47"/>
+      <c r="B25" s="48"/>
+      <c r="C25" s="48"/>
+      <c r="D25" s="48"/>
+      <c r="E25" s="48"/>
+      <c r="F25" s="48"/>
+      <c r="G25" s="48"/>
+      <c r="H25" s="48"/>
+      <c r="I25" s="48"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -2102,12 +2128,14 @@
     <hyperlink ref="K18" r:id="rId22" xr:uid="{BFEA52A5-CEF2-41E7-9E85-8378AD7B1600}"/>
     <hyperlink ref="K8" r:id="rId23" xr:uid="{F995CA6B-8EC8-4ADE-A3CD-293AAC6637F2}"/>
     <hyperlink ref="J8" r:id="rId24" xr:uid="{E6848423-59EE-45A3-B2DC-EA76691AD64F}"/>
+    <hyperlink ref="J9" r:id="rId25" xr:uid="{FCA6E7F1-9505-42AF-BE90-9F9094529FAA}"/>
+    <hyperlink ref="K9" r:id="rId26" xr:uid="{1CE8A5CF-2E51-430F-876E-3A5DE158F21D}"/>
   </hyperlinks>
   <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="300"/>
-  <drawing r:id="rId25"/>
+  <drawing r:id="rId27"/>
   <tableParts count="1">
-    <tablePart r:id="rId26"/>
+    <tablePart r:id="rId28"/>
   </tableParts>
 </worksheet>
 </file>

</xml_diff>